<commit_message>
update immediate feedback tests code base
</commit_message>
<xml_diff>
--- a/inst/extdata/teams_template.xlsx
+++ b/inst/extdata/teams_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sk/Dropbox/Tools/software/R/tbltools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23859C9B-B3C4-EF47-962C-1BA3F21473AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC76FB5-A20D-034F-A85E-9425D7273EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11400" yWindow="2240" windowWidth="25360" windowHeight="18780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3440" yWindow="460" windowWidth="25360" windowHeight="16580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="teams" sheetId="1" r:id="rId1"/>
@@ -73,9 +73,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>team</t>
-  </si>
-  <si>
     <t>1234</t>
   </si>
   <si>
@@ -88,7 +85,10 @@
     <t>4242</t>
   </si>
   <si>
-    <t>Don't Panic</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Team Don't Panic</t>
   </si>
 </sst>
 </file>
@@ -580,7 +580,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -591,18 +591,18 @@
   <sheetData>
     <row r="1" spans="1:2" s="4" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -610,7 +610,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>